<commit_message>
v1.1 add more test cases
add more test cases according the reviewer comments on the previous version
</commit_message>
<xml_diff>
--- a/LH_TESTCASES/LH_TC_PUBLISH&UPLOAD.xlsx
+++ b/LH_TESTCASES/LH_TC_PUBLISH&UPLOAD.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\testing\iti\6_QA\workshop\pulled repo\Group-3-Learning-hub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\testing\iti\6_QA\workshop\pulled repo\Group-3-Learning-hub-dev\Group-3-Learning-hub-dev\LH_TESTCASES\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LH_TC_FEATURENAME" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="124">
   <si>
     <t>Preconditions</t>
   </si>
@@ -184,9 +184,6 @@
     <t>Controls ("Start/Stop," "Publish") are visible and functional.</t>
   </si>
   <si>
-    <t>Upload Valid Video File (≤100MB)</t>
-  </si>
-  <si>
     <t>File uploads successfully.</t>
   </si>
   <si>
@@ -196,16 +193,10 @@
     <t>File is rejected with error: "Max size: 100MB."</t>
   </si>
   <si>
-    <t>Upload Valid Audio File (≤20MB)</t>
-  </si>
-  <si>
     <t>Upload Invalid Audio File (&gt;20MB)</t>
   </si>
   <si>
     <t>File is rejected with error: "Max size: 20MB."</t>
-  </si>
-  <si>
-    <t>Verify Article Word Limit (≤1000 Words)</t>
   </si>
   <si>
     <t>Submission allowed.</t>
@@ -387,6 +378,73 @@
   </si>
   <si>
     <t>initial test cases for publish and upload feature</t>
+  </si>
+  <si>
+    <t>Upload Valid Video File (&lt;100MB)</t>
+  </si>
+  <si>
+    <t>Upload Valid Video File (=100MB)</t>
+  </si>
+  <si>
+    <t>1. Open publishing interface.
+2. Click "Upload Video."
+3. Select 100MB MP4 file.
+4. Click "Publish."</t>
+  </si>
+  <si>
+    <t>Valid Video: 100MB MP4</t>
+  </si>
+  <si>
+    <t>Upload Valid Audio File (&lt;20MB)</t>
+  </si>
+  <si>
+    <t>Upload Valid Audio File (=20MB)</t>
+  </si>
+  <si>
+    <t>1. Open publishing interface.
+2. Click "Upload Audio."
+3. Select 20MB MP3 file.
+4. Click "Publish."</t>
+  </si>
+  <si>
+    <t>Valid Audio: 20MB MP3</t>
+  </si>
+  <si>
+    <t>Verify Article Word Limit (=1000 Words)</t>
+  </si>
+  <si>
+    <t>Verify Article Word Limit (&lt;1000 Words)</t>
+  </si>
+  <si>
+    <t>1. Open publishing interface.
+2. Click "Publish Article."
+3. Enter 1000 words.
+4. Click "Publish."</t>
+  </si>
+  <si>
+    <t>Valid: 1000 words article</t>
+  </si>
+  <si>
+    <t>TC-PUB-017</t>
+  </si>
+  <si>
+    <t>TC-PUB-018</t>
+  </si>
+  <si>
+    <t>TC-PUB-019</t>
+  </si>
+  <si>
+    <t>V1.1</t>
+  </si>
+  <si>
+    <t>21/4/2025</t>
+  </si>
+  <si>
+    <t>22/4/2026</t>
+  </si>
+  <si>
+    <t>add more test cases according the reviewer 
+comments on the previous version</t>
   </si>
 </sst>
 </file>
@@ -482,7 +540,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -576,15 +634,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFA3A3A3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color theme="0"/>
       </left>
@@ -602,7 +651,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -643,7 +692,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -674,9 +723,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -694,13 +740,159 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="36">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1221,10 +1413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -1247,44 +1439,44 @@
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="34"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="33"/>
       <c r="E1" s="18"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="37"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="36"/>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="35" t="s">
-        <v>106</v>
-      </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="37"/>
+      <c r="B3" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="35"/>
+      <c r="D3" s="36"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="35" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="37"/>
+      <c r="B4" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="35"/>
+      <c r="D4" s="36"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -1339,10 +1531,10 @@
         <v>43</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F9" s="28" t="s">
         <v>44</v>
@@ -1367,10 +1559,10 @@
         <v>47</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F10" s="29" t="s">
         <v>44</v>
@@ -1395,10 +1587,10 @@
         <v>49</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F11" s="28" t="s">
         <v>44</v>
@@ -1423,10 +1615,10 @@
         <v>51</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F12" s="29" t="s">
         <v>44</v>
@@ -1448,19 +1640,19 @@
         <v>28</v>
       </c>
       <c r="C13" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="G13" s="28" t="s">
         <v>53</v>
-      </c>
-      <c r="D13" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="E13" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="F13" s="28" t="s">
-        <v>86</v>
-      </c>
-      <c r="G13" s="28" t="s">
-        <v>54</v>
       </c>
       <c r="H13" s="25"/>
       <c r="I13" s="27"/>
@@ -1469,54 +1661,54 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="69" x14ac:dyDescent="0.35">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="21" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="24" t="s">
-        <v>55</v>
+      <c r="C14" s="29" t="s">
+        <v>106</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="F14" s="29" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="H14" s="24"/>
+        <v>53</v>
+      </c>
+      <c r="H14" s="21"/>
       <c r="I14" s="23"/>
-      <c r="J14" s="24" t="s">
+      <c r="J14" s="21" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="69" x14ac:dyDescent="0.35">
       <c r="A15" s="25" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B15" s="25" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F15" s="28" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G15" s="28" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H15" s="25"/>
       <c r="I15" s="27"/>
@@ -1532,19 +1724,19 @@
         <v>33</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>58</v>
+        <v>109</v>
       </c>
       <c r="D16" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="E16" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="F16" s="29" t="s">
-        <v>89</v>
-      </c>
       <c r="G16" s="29" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="H16" s="24"/>
       <c r="I16" s="23"/>
@@ -1554,230 +1746,314 @@
     </row>
     <row r="17" spans="1:10" ht="69" x14ac:dyDescent="0.35">
       <c r="A17" s="25" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B17" s="25" t="s">
         <v>34</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>80</v>
+        <v>111</v>
       </c>
       <c r="F17" s="28" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="G17" s="28" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="H17" s="25"/>
       <c r="I17" s="27"/>
       <c r="J17" s="25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="86.25" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="69" x14ac:dyDescent="0.35">
       <c r="A18" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="37" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F18" s="29" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G18" s="29" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="H18" s="24"/>
       <c r="I18" s="23"/>
       <c r="J18" s="24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="69" x14ac:dyDescent="0.35">
+      <c r="A19" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" s="25"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="69" x14ac:dyDescent="0.35">
+      <c r="A20" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="F20" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="G20" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" s="21"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="86.25" x14ac:dyDescent="0.35">
+      <c r="A21" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="H21" s="25"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="86.25" x14ac:dyDescent="0.35">
+      <c r="A22" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="F22" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="G22" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="H22" s="24"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="86.25" x14ac:dyDescent="0.35">
+      <c r="A23" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="F23" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="G23" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="H23" s="25"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="30" customFormat="1" ht="69" x14ac:dyDescent="0.35">
+      <c r="A24" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="29" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="87" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="F19" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="G19" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="H19" s="24"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="24" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="86.25" x14ac:dyDescent="0.35">
-      <c r="A20" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="D20" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="E20" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="F20" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="G20" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="H20" s="25"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" s="30" customFormat="1" ht="69" x14ac:dyDescent="0.35">
-      <c r="A21" s="24" t="s">
+      <c r="D24" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="F24" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="G24" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="H24" s="21"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="69" x14ac:dyDescent="0.35">
+      <c r="A25" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="24" t="s">
+      <c r="B25" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="F25" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="G25" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="H25" s="25"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="69" x14ac:dyDescent="0.35">
+      <c r="A26" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C26" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="D21" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="E21" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="F21" s="29" t="s">
+      <c r="D26" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="F26" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="G26" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="H26" s="24"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="69" x14ac:dyDescent="0.35">
+      <c r="A27" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="F27" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="G21" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="H21" s="24"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="24" t="s">
+      <c r="G27" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="H27" s="25"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="25" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="69" x14ac:dyDescent="0.35">
-      <c r="A22" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="D22" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="E22" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="F22" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="G22" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="H22" s="25"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="69" x14ac:dyDescent="0.35">
-      <c r="A23" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="C23" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="E23" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="F23" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="G23" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="H23" s="24"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="69" x14ac:dyDescent="0.35">
-      <c r="A24" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="C24" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="D24" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="E24" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="F24" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="G24" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="H24" s="25"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="I25" s="20"/>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I28" s="20"/>
     </row>
   </sheetData>
   <autoFilter ref="A8:I9"/>
@@ -1787,92 +2063,92 @@
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
   </mergeCells>
-  <conditionalFormatting sqref="I25:I1048576">
-    <cfRule type="containsText" dxfId="21" priority="25" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",I25)))</formula>
+  <conditionalFormatting sqref="I28:I1048576">
+    <cfRule type="containsText" dxfId="35" priority="39" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",I28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="26" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",I25)))</formula>
+    <cfRule type="containsText" dxfId="34" priority="40" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",I28)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I9:I10 I12 I14 I16 I18:I19">
-    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="Fail">
+  <conditionalFormatting sqref="I9:I10 I12 I18">
+    <cfRule type="containsText" dxfId="33" priority="37" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="32" priority="38" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11">
-    <cfRule type="containsText" dxfId="17" priority="21" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="31" priority="35" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="22" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="30" priority="36" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I11)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
-    <cfRule type="containsText" dxfId="15" priority="19" operator="containsText" text="Fail">
+  <conditionalFormatting sqref="I17">
+    <cfRule type="containsText" dxfId="27" priority="31" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",I17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="32" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",I17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13:I14 I16">
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="20" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15">
-    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="18" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I15)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I17">
-    <cfRule type="containsText" dxfId="11" priority="15" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",I17)))</formula>
+  <conditionalFormatting sqref="I19:I20 I22">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",I19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="16" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",I17)))</formula>
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",I19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21">
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I21)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I20">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",I20)))</formula>
+  <conditionalFormatting sqref="I27">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",I27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",I20)))</formula>
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",I27)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I23">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="Fail">
+  <conditionalFormatting sqref="I23:I24 I26">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I23)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I22">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",I22)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",I22)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I24">
+  <conditionalFormatting sqref="I25">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",I24)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Fail",I25)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",I24)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Pass",I25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -1889,8 +2165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1923,18 +2199,25 @@
         <v>20</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="D2" s="13">
-        <f ca="1">TODAY()</f>
-        <v>45766</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
+        <v>104</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="9" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="4" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>

</xml_diff>

<commit_message>
v1.2 modify some test cases
modify some test cases according to the latest version of SRS v1.4
</commit_message>
<xml_diff>
--- a/LH_TESTCASES/LH_TC_PUBLISH&UPLOAD.xlsx
+++ b/LH_TESTCASES/LH_TC_PUBLISH&UPLOAD.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="127">
   <si>
     <t>Preconditions</t>
   </si>
@@ -190,15 +190,9 @@
     <t>Upload Invalid Video File (&gt;100MB)</t>
   </si>
   <si>
-    <t>File is rejected with error: "Max size: 100MB."</t>
-  </si>
-  <si>
     <t>Upload Invalid Audio File (&gt;20MB)</t>
   </si>
   <si>
-    <t>File is rejected with error: "Max size: 20MB."</t>
-  </si>
-  <si>
     <t>Submission allowed.</t>
   </si>
   <si>
@@ -206,9 +200,6 @@
   </si>
   <si>
     <t>Verify Article Word Limit (&gt;1000 Words)</t>
-  </si>
-  <si>
-    <t>Submission blocked.</t>
   </si>
   <si>
     <t>Validate Valid Video Format (.mp4 Only)</t>
@@ -440,11 +431,29 @@
     <t>21/4/2025</t>
   </si>
   <si>
-    <t>22/4/2026</t>
-  </si>
-  <si>
     <t>add more test cases according the reviewer 
 comments on the previous version</t>
+  </si>
+  <si>
+    <t>Submission blocked.and error message of "article body exceeds 1000 words"</t>
+  </si>
+  <si>
+    <t>File is rejected, ,with error message of: "Max size: 100MB."</t>
+  </si>
+  <si>
+    <t>File is rejected, with error message of : "Max size: 20MB."</t>
+  </si>
+  <si>
+    <t>V1.2</t>
+  </si>
+  <si>
+    <t>modify some test cases according to the latest version of SRS v1.4</t>
+  </si>
+  <si>
+    <t>26/4/2025</t>
+  </si>
+  <si>
+    <t>22/4/2025</t>
   </si>
 </sst>
 </file>
@@ -723,6 +732,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -740,159 +755,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="22">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1415,8 +1284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="C22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -1439,44 +1308,44 @@
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="33"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="35"/>
       <c r="E1" s="18"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="36"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="38"/>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="34" t="s">
-        <v>103</v>
-      </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="36"/>
+      <c r="B3" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="37"/>
+      <c r="D3" s="38"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="36"/>
+      <c r="B4" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="37"/>
+      <c r="D4" s="38"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -1531,10 +1400,10 @@
         <v>43</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F9" s="28" t="s">
         <v>44</v>
@@ -1559,10 +1428,10 @@
         <v>47</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F10" s="29" t="s">
         <v>44</v>
@@ -1587,10 +1456,10 @@
         <v>49</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F11" s="28" t="s">
         <v>44</v>
@@ -1615,10 +1484,10 @@
         <v>51</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F12" s="29" t="s">
         <v>44</v>
@@ -1640,16 +1509,16 @@
         <v>28</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G13" s="28" t="s">
         <v>53</v>
@@ -1668,16 +1537,16 @@
         <v>30</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F14" s="29" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G14" s="29" t="s">
         <v>53</v>
@@ -1699,16 +1568,16 @@
         <v>54</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F15" s="28" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G15" s="28" t="s">
-        <v>55</v>
+        <v>121</v>
       </c>
       <c r="H15" s="25"/>
       <c r="I15" s="27"/>
@@ -1724,16 +1593,16 @@
         <v>33</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D16" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="29" t="s">
         <v>82</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="F16" s="29" t="s">
-        <v>85</v>
       </c>
       <c r="G16" s="29" t="s">
         <v>53</v>
@@ -1752,16 +1621,16 @@
         <v>34</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F17" s="28" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G17" s="28" t="s">
         <v>53</v>
@@ -1776,23 +1645,23 @@
       <c r="A18" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="31" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F18" s="29" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G18" s="29" t="s">
-        <v>57</v>
+        <v>122</v>
       </c>
       <c r="H18" s="24"/>
       <c r="I18" s="23"/>
@@ -1808,24 +1677,24 @@
         <v>37</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F19" s="28" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G19" s="28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H19" s="25"/>
       <c r="I19" s="27"/>
       <c r="J19" s="25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="69" x14ac:dyDescent="0.35">
@@ -1836,24 +1705,24 @@
         <v>39</v>
       </c>
       <c r="C20" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="F20" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="D20" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>115</v>
-      </c>
-      <c r="F20" s="29" t="s">
-        <v>116</v>
-      </c>
       <c r="G20" s="29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H20" s="21"/>
       <c r="I20" s="23"/>
       <c r="J20" s="21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="86.25" x14ac:dyDescent="0.35">
@@ -1864,24 +1733,24 @@
         <v>40</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F21" s="28" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G21" s="28" t="s">
-        <v>61</v>
+        <v>120</v>
       </c>
       <c r="H21" s="25"/>
       <c r="I21" s="27"/>
       <c r="J21" s="25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="86.25" x14ac:dyDescent="0.35">
@@ -1889,27 +1758,27 @@
         <v>35</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C22" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="F22" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="D22" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="F22" s="29" t="s">
-        <v>97</v>
-      </c>
       <c r="G22" s="29" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H22" s="24"/>
       <c r="I22" s="23"/>
       <c r="J22" s="24" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="86.25" x14ac:dyDescent="0.35">
@@ -1917,27 +1786,27 @@
         <v>35</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C23" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="F23" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="D23" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="E23" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="F23" s="28" t="s">
-        <v>102</v>
-      </c>
       <c r="G23" s="28" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H23" s="25"/>
       <c r="I23" s="27"/>
       <c r="J23" s="25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="30" customFormat="1" ht="69" x14ac:dyDescent="0.35">
@@ -1945,19 +1814,19 @@
         <v>38</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F24" s="29" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G24" s="29" t="s">
         <v>53</v>
@@ -1973,22 +1842,22 @@
         <v>38</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F25" s="28" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G25" s="28" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H25" s="25"/>
       <c r="I25" s="27"/>
@@ -2001,19 +1870,19 @@
         <v>41</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F26" s="29" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G26" s="29" t="s">
         <v>53</v>
@@ -2029,22 +1898,22 @@
         <v>41</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F27" s="28" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G27" s="28" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H27" s="25"/>
       <c r="I27" s="27"/>
@@ -2064,34 +1933,34 @@
     <mergeCell ref="B4:D4"/>
   </mergeCells>
   <conditionalFormatting sqref="I28:I1048576">
-    <cfRule type="containsText" dxfId="35" priority="39" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="21" priority="39" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="40" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="20" priority="40" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:I10 I12 I18">
-    <cfRule type="containsText" dxfId="33" priority="37" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="19" priority="37" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="38" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="18" priority="38" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11">
-    <cfRule type="containsText" dxfId="31" priority="35" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="17" priority="35" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="36" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="16" priority="36" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17">
-    <cfRule type="containsText" dxfId="27" priority="31" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="15" priority="31" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="32" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="14" priority="32" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I17)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2166,7 +2035,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2199,31 +2068,39 @@
         <v>20</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="9" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="9" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
+      <c r="B4" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="5" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>

</xml_diff>